<commit_message>
corrections colorbars and mainAF
</commit_message>
<xml_diff>
--- a/ARM_empirical_factors.xlsx
+++ b/ARM_empirical_factors.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clara/Documents/Work/CEREGE/PmagAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8956EB97-6788-9E4A-8811-AB27FB8ADC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E07BB-D2CC-DD4D-BDA7-CAD8FD86A501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="25040" windowHeight="13860" activeTab="2" xr2:uid="{EB24B50E-6652-BA4F-A7E9-56E28C5E96F3}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="25040" windowHeight="13860" xr2:uid="{EB24B50E-6652-BA4F-A7E9-56E28C5E96F3}"/>
   </bookViews>
   <sheets>
     <sheet name="CRM magnetite" sheetId="1" r:id="rId1"/>
     <sheet name="TRM magnetite" sheetId="2" r:id="rId2"/>
     <sheet name="TRM FeNi" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -523,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B756FA-640A-A040-BD64-B72C28CCDB95}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,6 +1164,9 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3145,7 +3158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B019BD24-9C7F-F849-AB2F-C86EE72B47B1}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>